<commit_message>
0429 : use case diagram, requirment list에 삭제 추가
</commit_message>
<xml_diff>
--- a/Requirement List & Actor Description.xlsx
+++ b/Requirement List & Actor Description.xlsx
@@ -3,7 +3,7 @@
 <x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:fileVersion appName="HCell" lastEdited="9.0" lowestEdited="9.0" rupBuild="0.568"/>
   <x:bookViews>
-    <x:workbookView xWindow="0" yWindow="0" windowWidth="28395" windowHeight="12210" activeTab="2"/>
+    <x:workbookView xWindow="0" yWindow="0" windowWidth="28395" windowHeight="12120" activeTab="1"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Actor Description" sheetId="1" r:id="rId4"/>
@@ -15,243 +15,249 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="79">
+<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="81">
+  <x:si>
+    <x:t>판매 의류 조회를 통해 얻은 판매의류 리스트에서 특정 상품을 선택한 후에 그 상품에 대한 모든 항목을 수정</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상품 구매 시 상품에 할당된 추가상품을 선택하여 추가 상품의 금액만큼 증가된 가격으로 구매할 수 있음</x:t>
+  </x:si>
   <x:si>
     <x:t>회원가입 버튼을 눌러 회원 정보(이름,주민번호,주소,이메일,ID,PW)를 입력하여 회원가입을 진행 후, 사용자에게 의류 쇼핑 사이트 사용 권한을 부여</x:t>
   </x:si>
   <x:si>
+    <x:t>의류 쇼핑 사이트에 회원가입을 하지 않아 사용 권한이 없는 고객</x:t>
+  </x:si>
+  <x:si>
+    <x:t>회원 가입시 중복 ID, 비밀번호 기준 등 유효성 검사 시행</x:t>
+  </x:si>
+  <x:si>
+    <x:t>추가상품 구매 시 기존상품과 가격이 합산되어 결제되어야 함</x:t>
+  </x:si>
+  <x:si>
+    <x:t>구매한 상품에 대한 환불 신청은 구매 날짜로부터 4주 이내여야함</x:t>
+  </x:si>
+  <x:si>
+    <x:t>로그아웃 버튼을 눌러 사용자 인증 해제 후 프로그램 자동 종료</x:t>
+  </x:si>
+  <x:si>
+    <x:t>결제 시 남은 포인트가 3000점 이상일 경우 포인트 사용 버튼을 눌러 포인트를 사용할 수 있다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>평균 구매 만족도순 정렬 버튼을 누르면 상품 정보 조회 리스트의 정렬 기준을 평균 구매만족도로 바꿈</x:t>
+  </x:si>
+  <x:si>
+    <x:t>의류 쇼핑 사이트에서 사용자가 상품을 구매 시 자동으로 결제금액의 1%를 포인트로 적립해주는 이벤트</x:t>
+  </x:si>
+  <x:si>
+    <x:t>사용자가 상품 환불 신청 시 자동으로 소모한 포인트 반환과 택배사에 물품 수거 신청을 보내는 이벤트</x:t>
+  </x:si>
+  <x:si>
+    <x:t>매월 말 모든 회원들에게 그 달에 대한 판매 및 구매 통계 정보를 이메일로 자동 공지하는 이벤트</x:t>
+  </x:si>
+  <x:si>
     <x:t>판매할 의류에 대한 정보(상품명, 제작회사명, 가격, 수량, 추가상품, 추가상품 가격, 판매종료일)를 저장하는 데이터베이스</x:t>
   </x:si>
   <x:si>
+    <x:t>통계보기 버튼을 눌러 회원이 판매한 상품에 대한 총액 및 평균 구매만족도와 구매한 상품에 대한 총액 및 평균 구매만족도를 출력. 삭제된 구매 내역은 통계에서 제외함</x:t>
+  </x:si>
+  <x:si>
+    <x:t>물품 수거 신청 요청을 받음</x:t>
+  </x:si>
+  <x:si>
+    <x:t>판매 완료된 상품 내역 조회</x:t>
+  </x:si>
+  <x:si>
+    <x:t>평균 구매 만족도순 정렬</x:t>
+  </x:si>
+  <x:si>
+    <x:t>매월 말일에 모든 회원들에게 그 달에 대한 판매 및 구매 통계 정보를 이메일로 공지함</x:t>
+  </x:si>
+  <x:si>
+    <x:t>의류 쇼핑 사이트에 회원가입을 하여 로그인을 통해 시스템을 사용할 권한이 있는 고객</x:t>
+  </x:si>
+  <x:si>
+    <x:t>구매내역 조회 시 하나의 상품을 선택하여 구매만족도를 평가할 수 있음</x:t>
+  </x:si>
+  <x:si>
+    <x:t>환불 신청한 상품에 대해 택배사에 자동으로 물품 수거 신청이 요청됨</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상품 환불 시 포인트를 사용하여 결제 했다면 사용한 포인트를 돌려받음</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ID와 PW를 입력하여 사용자 인증을 통해 클라이언트의 접속 허용</x:t>
+  </x:si>
+  <x:si>
+    <x:t>판매 의류 조회 버튼을 눌러 자신이 등록한 의류 상품의 리스트 조회</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상품 정보 조회 리스트에서 원하는 상품을 선택하면 해당 상품의 상세한 정보(상품명, 제작회사명, 가격, 수량, 추가상품, 추가상품 가격, 판매종료일, 평균 구매만족도)가 출력되며 즉시 결제한 후 구매할 수 있음</x:t>
+  </x:si>
+  <x:si>
+    <x:t>로그인</x:t>
+  </x:si>
+  <x:si>
+    <x:t>No.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>회원</x:t>
+  </x:si>
+  <x:si>
+    <x:t>사용자</x:t>
+  </x:si>
+  <x:si>
+    <x:t>결제</x:t>
+  </x:si>
+  <x:si>
+    <x:t>택배사</x:t>
+  </x:si>
+  <x:si>
+    <x:t>비회원</x:t>
+  </x:si>
+  <x:si>
+    <x:t>구매내역 조회 시 3개월이 지난 구매 거래내역은 구매내역삭제 버튼을 눌러 임의로 삭제하며, 그 이전의 구매내역은 임의로 삭제할 수 없음.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>검색 조건(상품명, 평균 구매만족도) 중 하나를 선택하여 입력하면 이에 해당하는 상품 리스트를 상품명의 오름차순으로 출력하여 알아보기 쉽게 함</x:t>
+  </x:si>
+  <x:si>
+    <x:t>판매한 상품에 대한 총액 및 평균 구매만족도와 구매한 상품에 대한 총액 및 평균 구매만족도에 대한 통계를 구할 수 있는 데이터베이스 환경</x:t>
+  </x:si>
+  <x:si>
+    <x:t>구매내역 조회 버튼을 눌러 구매내역 정보(상품명, 제작회사명, 판매자, 가격, 평균 구매만족도, 구매일)를 조회할 수 있다. 이 때 상품명의 오름차순으로 정렬해서 출력함</x:t>
+  </x:si>
+  <x:si>
+    <x:t>프로그램을 구동하는 서버의 안정성과 속도가 보장되어야함</x:t>
+  </x:si>
+  <x:si>
+    <x:t>결제 시 구매대금이 판매자에게 올바르게 전달되어야함</x:t>
+  </x:si>
+  <x:si>
+    <x:t>회원이 판매할 상품에 대한 정보(상품명, 제작회사명, 가격, 수량, 추가상품, 추가상품 가격, 판매종료일)를 입력하여 프로그램에 등록함</x:t>
+  </x:si>
+  <x:si>
+    <x:t>결제 시 결제 대금의 1%를 포인트로 자동 적립</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6개월이 지난 구매 거래내역은 자동 삭제됨.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>개인정보를 저장하고 관리하는 데이터베이스와 서버</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Actor Description</x:t>
+  </x:si>
+  <x:si>
+    <x:t>매월 말일 이메일 발송 event</x:t>
+  </x:si>
+  <x:si>
+    <x:t>개발 팀 내 버전컨트롤을 위한 툴</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Requirement List</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상품 판매 및 구매 통계 출력</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상품 구매내역에서 구입 후 6개월이 지난 거래내역을 자동으로 삭제하는 이벤트</x:t>
+  </x:si>
+  <x:si>
     <x:t>환불 신청 시 택배사에 자동으로 물품 수거 신청할 수 있도록 인터페이스 확립</x:t>
   </x:si>
   <x:si>
-    <x:t>상품 구매내역에서 구입 후 6개월이 지난 거래내역을 자동으로 삭제하는 이벤트</x:t>
-  </x:si>
-  <x:si>
-    <x:t>상품 구매 시 상품에 할당된 추가상품을 선택하여 추가 상품의 금액만큼 증가된 가격으로 구매할 수 있음</x:t>
-  </x:si>
-  <x:si>
-    <x:t>판매 의류 조회를 통해 얻은 판매의류 리스트에서 특정 상품을 선택한 후에 그 상품에 대한 모든 항목을 수정</x:t>
-  </x:si>
-  <x:si>
-    <x:t>통계보기 버튼을 눌러 회원이 판매한 상품에 대한 총액 및 평균 구매만족도와 구매한 상품에 대한 총액 및 평균 구매만족도를 출력. 삭제된 구매 내역은 통계에서 제외함</x:t>
-  </x:si>
-  <x:si>
-    <x:t>매월 말일에 모든 회원들에게 그 달에 대한 판매 및 구매 통계 정보를 이메일로 공지함</x:t>
-  </x:si>
-  <x:si>
-    <x:t>의류 쇼핑 사이트에 회원가입을 하여 로그인을 통해 시스템을 사용할 권한이 있는 고객</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ID와 PW를 입력하여 사용자 인증을 통해 클라이언트의 접속 허용</x:t>
-  </x:si>
-  <x:si>
-    <x:t>판매 의류 조회 버튼을 눌러 자신이 등록한 의류 상품의 리스트 조회</x:t>
-  </x:si>
-  <x:si>
-    <x:t>환불 신청한 상품에 대해 택배사에 자동으로 물품 수거 신청이 요청됨</x:t>
-  </x:si>
-  <x:si>
-    <x:t>상품 환불 시 포인트를 사용하여 결제 했다면 사용한 포인트를 돌려받음</x:t>
-  </x:si>
-  <x:si>
-    <x:t>구매내역 조회 시 하나의 상품을 선택하여 구매만족도를 평가할 수 있음</x:t>
-  </x:si>
-  <x:si>
-    <x:t>회원이 판매할 상품에 대한 정보(상품명, 제작회사명, 가격, 수량, 추가상품, 추가상품 가격, 판매종료일)를 입력하여 프로그램에 등록함</x:t>
-  </x:si>
-  <x:si>
-    <x:t>개발 팀 내 버전컨트롤을 위한 툴</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Requirement List</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Actor Description</x:t>
-  </x:si>
-  <x:si>
-    <x:t>매월 말일 이메일 발송 event</x:t>
-  </x:si>
-  <x:si>
-    <x:t>상품 판매 및 구매 통계 출력</x:t>
-  </x:si>
-  <x:si>
     <x:t>판매 완료된 상품 내역 조회 버튼을 눌러 회원의 판매 상품 중 판매 종료일이 지났거나 남은 수량이 0이 된 상품을 조회</x:t>
   </x:si>
   <x:si>
-    <x:t>프로그램을 구동하는 서버의 안정성과 속도가 보장되어야함</x:t>
-  </x:si>
-  <x:si>
-    <x:t>결제 시 구매대금이 판매자에게 올바르게 전달되어야함</x:t>
-  </x:si>
-  <x:si>
-    <x:t>구매내역 조회 버튼을 눌러 구매내역 정보(상품명, 제작회사명, 판매자, 가격, 평균 구매만족도, 구매일)를 조회할 수 있다. 이 때 상품명의 오름차순으로 정렬해서 출력함</x:t>
-  </x:si>
-  <x:si>
-    <x:t>결제 시 남은 포인트가 3000점 이상일 경우 포인트 사용 버튼을 눌러 포인트를 사용할 수 있다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>평균 구매 만족도순 정렬 버튼을 누르면 상품 정보 조회 리스트의 정렬 기준을 평균 구매만족도로 바꿈</x:t>
-  </x:si>
-  <x:si>
-    <x:t>의류 쇼핑 사이트에서 사용자가 상품을 구매 시 자동으로 결제금액의 1%를 포인트로 적립해주는 이벤트</x:t>
-  </x:si>
-  <x:si>
-    <x:t>사용자가 상품 환불 신청 시 자동으로 소모한 포인트 반환과 택배사에 물품 수거 신청을 보내는 이벤트</x:t>
-  </x:si>
-  <x:si>
-    <x:t>매월 말 모든 회원들에게 그 달에 대한 판매 및 구매 통계 정보를 이메일로 자동 공지하는 이벤트</x:t>
-  </x:si>
-  <x:si>
-    <x:t>결제 시 결제 대금의 1%를 포인트로 자동 적립</x:t>
-  </x:si>
-  <x:si>
-    <x:t>6개월이 지난 구매 거래내역은 자동 삭제됨.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>개인정보를 저장하고 관리하는 데이터베이스와 서버</x:t>
-  </x:si>
-  <x:si>
-    <x:t>의류 쇼핑 사이트에 회원가입을 하지 않아 사용 권한이 없는 고객</x:t>
-  </x:si>
-  <x:si>
-    <x:t>로그아웃 버튼을 눌러 사용자 인증 해제 후 프로그램 자동 종료</x:t>
-  </x:si>
-  <x:si>
-    <x:t>회원 가입시 중복 ID, 비밀번호 기준 등 유효성 검사 시행</x:t>
-  </x:si>
-  <x:si>
-    <x:t>추가상품 구매 시 기존상품과 가격이 합산되어 결제되어야 함</x:t>
-  </x:si>
-  <x:si>
-    <x:t>구매한 상품에 대한 환불 신청은 구매 날짜로부터 4주 이내여야함</x:t>
-  </x:si>
-  <x:si>
-    <x:t>판매한 상품에 대한 총액 및 평균 구매만족도와 구매한 상품에 대한 총액 및 평균 구매만족도에 대한 통계를 구할 수 있는 데이터베이스 환경</x:t>
-  </x:si>
-  <x:si>
-    <x:t>구매내역 조회 시 3개월이 지난 구매 거래내역은 구매내역삭제 버튼을 눌러 임의로 삭제하며, 그 이전의 구매내역은 임의로 삭제할 수 없음.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>검색 조건(상품명, 평균 구매만족도) 중 하나를 선택하여 입력하면 이에 해당하는 상품 리스트를 상품명의 오름차순으로 출력하여 알아보기 쉽게 함</x:t>
+    <x:t>판매 의류 등록</x:t>
+  </x:si>
+  <x:si>
+    <x:t>판매 의류 조회</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상품 정보 조회</x:t>
+  </x:si>
+  <x:si>
+    <x:t>판매 의류 수정</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Use Case(s)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>구매 만족도 평가</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Requirement</x:t>
+  </x:si>
+  <x:si>
+    <x:t>use case</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상품 구매내역 삭제</x:t>
+  </x:si>
+  <x:si>
+    <x:t>물품 수거 신청</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상품 구매 event</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상품 환불 event</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Description</x:t>
+  </x:si>
+  <x:si>
+    <x:t>판매 의류 삭제</x:t>
+  </x:si>
+  <x:si>
+    <x:t>포인트 적립</x:t>
+  </x:si>
+  <x:si>
+    <x:t>추가상품구매</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상품 환불</x:t>
+  </x:si>
+  <x:si>
+    <x:t>포인트 환불</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Actor</x:t>
+  </x:si>
+  <x:si>
+    <x:t>구매내역 조회</x:t>
+  </x:si>
+  <x:si>
+    <x:t>회원가입</x:t>
+  </x:si>
+  <x:si>
+    <x:t>회원탈퇴</x:t>
+  </x:si>
+  <x:si>
+    <x:t>포인트 사용</x:t>
+  </x:si>
+  <x:si>
+    <x:t>로그아웃</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6개월이 지난 구매내역은 자동으로 삭제함</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6개월이 지난 거래 내역 삭제 event</x:t>
+  </x:si>
+  <x:si>
+    <x:t>등록한 상품이 하나도 없는 회원은 회원 탈퇴 버튼을 눌러 회원의 시스템 사용 권한 소멸</x:t>
+  </x:si>
+  <x:si>
+    <x:t>의류 쇼핑 사이트의 회원으로서 시스템의 모든 기능(판매, 구매 등)을 사용할 수 있는 고객</x:t>
   </x:si>
   <x:si>
     <x:t>구매내역 조회 시 구입 후 4주가 지나지 않은 하나의 상품을 선택하여 환불을 신청할 수 있음</x:t>
   </x:si>
   <x:si>
-    <x:t>등록한 상품이 하나도 없는 회원은 회원 탈퇴 버튼을 눌러 회원의 시스템 사용 권한 소멸</x:t>
-  </x:si>
-  <x:si>
-    <x:t>의류 쇼핑 사이트의 회원으로서 시스템의 모든 기능(판매, 구매 등)을 사용할 수 있는 고객</x:t>
-  </x:si>
-  <x:si>
-    <x:t>포인트 적립</x:t>
-  </x:si>
-  <x:si>
-    <x:t>추가상품구매</x:t>
-  </x:si>
-  <x:si>
-    <x:t>상품 환불</x:t>
-  </x:si>
-  <x:si>
-    <x:t>포인트 환불</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Actor</x:t>
-  </x:si>
-  <x:si>
-    <x:t>구매내역 조회</x:t>
-  </x:si>
-  <x:si>
-    <x:t>회원가입</x:t>
-  </x:si>
-  <x:si>
-    <x:t>회원탈퇴</x:t>
-  </x:si>
-  <x:si>
-    <x:t>로그아웃</x:t>
-  </x:si>
-  <x:si>
-    <x:t>포인트 사용</x:t>
-  </x:si>
-  <x:si>
-    <x:t>상품 정보 조회 리스트에서 원하는 상품을 선택하면 해당 상품의 상세한 정보(상품명, 제작회사명, 가격, 수량, 추가상품, 추가상품 가격, 판매종료일, 평균 구매만족도)가 출력되며 즉시 결제한 후 구매할 수 있음</x:t>
-  </x:si>
-  <x:si>
-    <x:t>6개월이 지난 구매내역은 자동으로 삭제함</x:t>
-  </x:si>
-  <x:si>
-    <x:t>6개월이 지난 거래 내역 삭제 event</x:t>
-  </x:si>
-  <x:si>
-    <x:t>로그인</x:t>
-  </x:si>
-  <x:si>
-    <x:t>No.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>결제</x:t>
-  </x:si>
-  <x:si>
-    <x:t>회원</x:t>
-  </x:si>
-  <x:si>
-    <x:t>택배사</x:t>
-  </x:si>
-  <x:si>
-    <x:t>사용자</x:t>
-  </x:si>
-  <x:si>
-    <x:t>비회원</x:t>
-  </x:si>
-  <x:si>
-    <x:t>평균 구매 만족도순 정렬</x:t>
-  </x:si>
-  <x:si>
-    <x:t>물품 수거 신청 요청을 받음</x:t>
-  </x:si>
-  <x:si>
-    <x:t>판매 완료된 상품 내역 조회</x:t>
-  </x:si>
-  <x:si>
-    <x:t>판매 의류 등록</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Use Case(s)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Requirement</x:t>
-  </x:si>
-  <x:si>
-    <x:t>판매 의류 조회</x:t>
-  </x:si>
-  <x:si>
-    <x:t>상품 정보 조회</x:t>
-  </x:si>
-  <x:si>
-    <x:t>판매 의류 수정</x:t>
-  </x:si>
-  <x:si>
-    <x:t>구매 만족도 평가</x:t>
-  </x:si>
-  <x:si>
-    <x:t>use case</x:t>
-  </x:si>
-  <x:si>
-    <x:t>상품 구매내역 삭제</x:t>
-  </x:si>
-  <x:si>
-    <x:t>물품 수거 신청</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Description</x:t>
-  </x:si>
-  <x:si>
-    <x:t>상품 환불 event</x:t>
-  </x:si>
-  <x:si>
-    <x:t>상품 구매 event</x:t>
+    <x:t>판매 의류 조회를 통해 얻은 판매의류 리스트에서 특정 상품을 선택한 후에 그 상품을 삭제</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -542,7 +548,6 @@
           <x:font hs:extension="1">
             <x:color rgb="ff000000"/>
             <x:b val="1"/>
-            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -587,7 +592,6 @@
           <x:font hs:extension="1">
             <x:color rgb="ff000000"/>
             <x:b val="1"/>
-            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -664,7 +668,6 @@
           <x:font hs:extension="1">
             <x:color rgb="ff000000"/>
             <x:b val="1"/>
-            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -703,7 +706,6 @@
           <x:font hs:extension="1">
             <x:color rgb="ff000000"/>
             <x:b val="1"/>
-            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -726,7 +728,6 @@
           <x:font hs:extension="1">
             <x:color rgb="ff000000"/>
             <x:b val="1"/>
-            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -759,7 +760,6 @@
           <x:font hs:extension="1">
             <x:color rgb="ff000000"/>
             <x:b val="1"/>
-            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -807,7 +807,6 @@
         <x:dxf hs:applyExtension="1">
           <x:font hs:extension="1">
             <x:color rgb="ff000000"/>
-            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -863,7 +862,6 @@
           <x:font hs:extension="1">
             <x:color rgb="ffffffff"/>
             <x:b val="1"/>
-            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -898,7 +896,6 @@
           <x:font hs:extension="1">
             <x:color rgb="ff000000"/>
             <x:b val="1"/>
-            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -931,7 +928,6 @@
           <x:font hs:extension="1">
             <x:color rgb="ff000000"/>
             <x:b val="1"/>
-            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -954,7 +950,6 @@
           <x:font hs:extension="1">
             <x:color rgb="ff000000"/>
             <x:b val="1"/>
-            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -988,7 +983,7 @@
       </x:fill>
     </x:dxf>
   </x:dxfs>
-  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+  <x:tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <x:tableStyle name="PivotStyleLight16" pivot="1" table="0" count="11">
       <x:tableStyleElement type="headerRow" size="1" dxfId="0"/>
       <x:tableStyleElement type="totalRow" size="1" dxfId="1"/>
@@ -1312,7 +1307,7 @@
       <x:selection activeCell="E9" activeCellId="0" sqref="E9:E9"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="21.600000000000001"/>
+  <x:sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.550000000000001"/>
   <x:cols>
     <x:col min="1" max="1" width="8.796875" style="4"/>
     <x:col min="2" max="2" width="25.3984375" style="3" customWidth="1"/>
@@ -1320,117 +1315,117 @@
     <x:col min="4" max="16384" width="8.796875" style="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:3" customHeight="1">
+    <x:row r="1" spans="1:3" ht="21.600000000000001" customHeight="1">
       <x:c r="A1" s="14" t="s">
-        <x:v>17</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="B1" s="14"/>
       <x:c r="C1" s="14"/>
     </x:row>
-    <x:row r="2" spans="1:3" customHeight="1">
+    <x:row r="2" spans="1:3" ht="21.600000000000001" customHeight="1">
       <x:c r="A2" s="5" t="s">
-        <x:v>57</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="B2" s="12" t="s">
-        <x:v>47</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="C2" s="13" t="s">
-        <x:v>76</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:3" customHeight="1">
+        <x:v>63</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:3" ht="21.600000000000001" customHeight="1">
       <x:c r="A3" s="9">
         <x:v>1</x:v>
       </x:c>
       <x:c r="B3" s="11" t="s">
-        <x:v>62</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="C3" s="7" t="s">
-        <x:v>32</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:3" customHeight="1">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:3" ht="21.600000000000001" customHeight="1">
       <x:c r="A4" s="9">
         <x:v>2</x:v>
       </x:c>
       <x:c r="B4" s="11" t="s">
-        <x:v>59</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="C4" s="7" t="s">
-        <x:v>8</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:3" customHeight="1">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:3" ht="21.600000000000001" customHeight="1">
       <x:c r="A5" s="9">
         <x:v>3</x:v>
       </x:c>
       <x:c r="B5" s="11" t="s">
-        <x:v>61</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="C5" s="7" t="s">
-        <x:v>42</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:3" customHeight="1">
+        <x:v>78</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:3" ht="21.600000000000001" customHeight="1">
       <x:c r="A6" s="9">
         <x:v>4</x:v>
       </x:c>
       <x:c r="B6" s="11" t="s">
-        <x:v>78</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="C6" s="7" t="s">
-        <x:v>26</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:3" customHeight="1">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:3" ht="21.600000000000001" customHeight="1">
       <x:c r="A7" s="9">
         <x:v>5</x:v>
       </x:c>
       <x:c r="B7" s="11" t="s">
-        <x:v>77</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="C7" s="7" t="s">
-        <x:v>27</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:3" customHeight="1">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:3" ht="21.600000000000001" customHeight="1">
       <x:c r="A8" s="9">
         <x:v>6</x:v>
       </x:c>
       <x:c r="B8" s="11" t="s">
-        <x:v>60</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="C8" s="7" t="s">
-        <x:v>64</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:3" customHeight="1">
+        <x:v>15</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:3" ht="21.600000000000001" customHeight="1">
       <x:c r="A9" s="9">
         <x:v>7</x:v>
       </x:c>
       <x:c r="B9" s="11" t="s">
-        <x:v>55</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="C9" s="7" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="10" spans="1:3" customHeight="1">
+        <x:v>48</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:3" ht="21.600000000000001" customHeight="1">
       <x:c r="A10" s="9">
         <x:v>8</x:v>
       </x:c>
       <x:c r="B10" s="11" t="s">
-        <x:v>18</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="C10" s="7" t="s">
-        <x:v>28</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
   <x:mergeCells count="1">
     <x:mergeCell ref="A1:C1"/>
   </x:mergeCells>
-  <x:pageMargins left="0.69999998807907104" right="0.69999998807907104" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
+  <x:pageMargins left="0.69986110925674438" right="0.69986110925674438" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
   <x:pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="0" verticalDpi="0" copies="1"/>
 </x:worksheet>
 </file>
@@ -1440,11 +1435,11 @@
   <x:sheetPr codeName="Sheet2"/>
   <x:dimension ref="A1:C14"/>
   <x:sheetViews>
-    <x:sheetView topLeftCell="A1" zoomScaleNormal="100" workbookViewId="0">
-      <x:selection activeCell="B14" activeCellId="0" sqref="B14:B14"/>
+    <x:sheetView tabSelected="1" topLeftCell="A1" zoomScaleNormal="100" workbookViewId="0">
+      <x:selection activeCell="C12" activeCellId="0" sqref="C12:C12"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="31.050000000000001"/>
+  <x:sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.550000000000001"/>
   <x:cols>
     <x:col min="1" max="1" width="8.796875" style="4"/>
     <x:col min="2" max="2" width="73.3984375" style="3" customWidth="1"/>
@@ -1452,127 +1447,125 @@
     <x:col min="4" max="16384" width="8.796875" style="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:3" customHeight="1">
+    <x:row r="1" spans="1:3" ht="31.050000000000001" customHeight="1">
       <x:c r="A1" s="14" t="s">
-        <x:v>16</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="B1" s="14"/>
       <x:c r="C1" s="14"/>
     </x:row>
-    <x:row r="2" spans="1:3" customHeight="1">
+    <x:row r="2" spans="1:3" ht="31.050000000000001" customHeight="1">
       <x:c r="A2" s="5" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="B2" s="10" t="s">
         <x:v>57</x:v>
       </x:c>
-      <x:c r="B2" s="10" t="s">
-        <x:v>68</x:v>
-      </x:c>
       <x:c r="C2" s="5" t="s">
-        <x:v>73</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:3" customHeight="1">
+        <x:v>58</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:3" ht="31.050000000000001" customHeight="1">
       <x:c r="A3" s="9">
         <x:v>1</x:v>
       </x:c>
       <x:c r="B3" s="11" t="s">
-        <x:v>31</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="C3" s="7"/>
     </x:row>
-    <x:row r="4" spans="1:3" customHeight="1">
+    <x:row r="4" spans="1:3" ht="31.050000000000001" customHeight="1">
       <x:c r="A4" s="9">
         <x:v>2</x:v>
       </x:c>
       <x:c r="B4" s="11" t="s">
-        <x:v>34</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="C4" s="7"/>
     </x:row>
-    <x:row r="5" spans="1:3" customHeight="1">
+    <x:row r="5" spans="1:3" ht="31.050000000000001" customHeight="1">
       <x:c r="A5" s="9">
         <x:v>3</x:v>
       </x:c>
       <x:c r="B5" s="11" t="s">
-        <x:v>1</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="C5" s="7"/>
     </x:row>
-    <x:row r="6" spans="1:3" customHeight="1">
+    <x:row r="6" spans="1:3" ht="31.050000000000001" customHeight="1">
       <x:c r="A6" s="9">
         <x:v>4</x:v>
       </x:c>
       <x:c r="B6" s="11" t="s">
-        <x:v>15</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="C6" s="7"/>
     </x:row>
-    <x:row r="7" spans="1:3" customHeight="1">
+    <x:row r="7" spans="1:3" ht="31.050000000000001" customHeight="1">
       <x:c r="A7" s="9">
         <x:v>5</x:v>
       </x:c>
       <x:c r="B7" s="11" t="s">
-        <x:v>21</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="C7" s="7"/>
     </x:row>
-    <x:row r="8" spans="1:3" customHeight="1">
+    <x:row r="8" spans="1:3" ht="31.050000000000001" customHeight="1">
       <x:c r="A8" s="9">
         <x:v>6</x:v>
       </x:c>
       <x:c r="B8" s="11" t="s">
-        <x:v>22</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C8" s="7"/>
     </x:row>
-    <x:row r="9" spans="1:3" customHeight="1">
+    <x:row r="9" spans="1:3" ht="31.050000000000001" customHeight="1">
       <x:c r="A9" s="9">
         <x:v>7</x:v>
       </x:c>
       <x:c r="B9" s="11" t="s">
-        <x:v>35</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="C9" s="7"/>
     </x:row>
-    <x:row r="10" spans="1:3" customHeight="1">
+    <x:row r="10" spans="1:3" ht="31.050000000000001" customHeight="1">
       <x:c r="A10" s="9">
         <x:v>8</x:v>
       </x:c>
       <x:c r="B10" s="11" t="s">
-        <x:v>36</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="C10" s="7"/>
     </x:row>
-    <x:row r="11" spans="1:3" customHeight="1">
+    <x:row r="11" spans="1:3" ht="31.050000000000001" customHeight="1">
       <x:c r="A11" s="9">
         <x:v>9</x:v>
       </x:c>
       <x:c r="B11" s="11" t="s">
-        <x:v>54</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C11" s="7"/>
     </x:row>
-    <x:row r="12" spans="1:3" customHeight="1">
+    <x:row r="12" spans="1:3" ht="31.050000000000001" customHeight="1">
       <x:c r="A12" s="9">
         <x:v>10</x:v>
       </x:c>
       <x:c r="B12" s="11" t="s">
-        <x:v>2</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="C12" s="7"/>
     </x:row>
-    <x:row r="13" spans="1:3" customHeight="1">
+    <x:row r="13" spans="1:3" ht="31.050000000000001" customHeight="1">
       <x:c r="A13" s="9">
         <x:v>11</x:v>
       </x:c>
       <x:c r="B13" s="11" t="s">
-        <x:v>37</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="C13" s="7"/>
     </x:row>
-    <x:row r="14" spans="1:3" customHeight="1">
-      <x:c r="A14" s="9">
-        <x:v>12</x:v>
-      </x:c>
+    <x:row r="14" spans="1:3" ht="31.050000000000001" customHeight="1">
+      <x:c r="A14" s="9"/>
       <x:c r="B14" s="11"/>
       <x:c r="C14" s="7"/>
     </x:row>
@@ -1580,7 +1573,7 @@
   <x:mergeCells count="1">
     <x:mergeCell ref="A1:C1"/>
   </x:mergeCells>
-  <x:pageMargins left="0.69999998807907104" right="0.69999998807907104" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
+  <x:pageMargins left="0.69986110925674438" right="0.69986110925674438" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
   <x:pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="0" verticalDpi="0" copies="1"/>
 </x:worksheet>
 </file>
@@ -1588,13 +1581,13 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr codeName="Sheet3"/>
-  <x:dimension ref="A1:C25"/>
+  <x:dimension ref="A1:C26"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" topLeftCell="A1" zoomScaleNormal="100" workbookViewId="0">
-      <x:selection activeCell="D9" activeCellId="0" sqref="D9:D9"/>
+    <x:sheetView topLeftCell="A1" zoomScaleNormal="100" workbookViewId="0">
+      <x:selection activeCell="B10" activeCellId="0" sqref="B10:B10"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="31.050000000000001"/>
+  <x:sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.550000000000001"/>
   <x:cols>
     <x:col min="1" max="1" width="8.796875" style="4"/>
     <x:col min="2" max="2" width="78.5" style="2" customWidth="1"/>
@@ -1603,280 +1596,291 @@
     <x:col min="5" max="16384" width="8.796875" style="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:3" customHeight="1">
+    <x:row r="1" spans="1:3" ht="31.050000000000001" customHeight="1">
       <x:c r="A1" s="14" t="s">
-        <x:v>16</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="B1" s="14"/>
       <x:c r="C1" s="14"/>
     </x:row>
-    <x:row r="2" spans="1:3" customHeight="1">
+    <x:row r="2" spans="1:3" ht="31.050000000000001" customHeight="1">
       <x:c r="A2" s="5" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="B2" s="6" t="s">
         <x:v>57</x:v>
       </x:c>
-      <x:c r="B2" s="6" t="s">
-        <x:v>68</x:v>
-      </x:c>
       <x:c r="C2" s="5" t="s">
-        <x:v>67</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:3" customHeight="1">
+        <x:v>55</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:3" ht="31.050000000000001" customHeight="1">
       <x:c r="A3" s="9">
         <x:v>1</x:v>
       </x:c>
       <x:c r="B3" s="8" t="s">
-        <x:v>0</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="C3" s="7" t="s">
-        <x:v>49</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:3" customHeight="1">
+        <x:v>71</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:3" ht="31.050000000000001" customHeight="1">
       <x:c r="A4" s="9">
         <x:v>2</x:v>
       </x:c>
       <x:c r="B4" s="8" t="s">
-        <x:v>41</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="C4" s="7" t="s">
-        <x:v>50</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:3" customHeight="1">
+        <x:v>72</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:3" ht="31.050000000000001" customHeight="1">
       <x:c r="A5" s="9">
         <x:v>3</x:v>
       </x:c>
       <x:c r="B5" s="8" t="s">
-        <x:v>9</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="C5" s="7" t="s">
-        <x:v>56</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:3" customHeight="1">
+        <x:v>26</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:3" ht="31.050000000000001" customHeight="1">
       <x:c r="A6" s="9">
         <x:v>4</x:v>
       </x:c>
       <x:c r="B6" s="8" t="s">
-        <x:v>33</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="C6" s="7" t="s">
-        <x:v>51</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:3" customHeight="1">
+        <x:v>74</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:3" ht="31.050000000000001" customHeight="1">
       <x:c r="A7" s="9">
         <x:v>5</x:v>
       </x:c>
       <x:c r="B7" s="8" t="s">
-        <x:v>14</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="C7" s="7" t="s">
-        <x:v>66</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:3" customHeight="1">
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:3" ht="31.050000000000001" customHeight="1">
       <x:c r="A8" s="9">
         <x:v>6</x:v>
       </x:c>
       <x:c r="B8" s="8" t="s">
-        <x:v>10</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="C8" s="7" t="s">
-        <x:v>69</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:3" customHeight="1">
+        <x:v>52</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:3" ht="31.050000000000001" customHeight="1">
       <x:c r="A9" s="9">
         <x:v>7</x:v>
       </x:c>
       <x:c r="B9" s="8" t="s">
-        <x:v>5</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="C9" s="7" t="s">
-        <x:v>71</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="10" spans="1:3" customHeight="1">
+        <x:v>54</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:3" s="1" customFormat="1" ht="31.050000000000001" customHeight="1">
       <x:c r="A10" s="9">
         <x:v>8</x:v>
       </x:c>
       <x:c r="B10" s="8" t="s">
-        <x:v>20</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="C10" s="7" t="s">
-        <x:v>65</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="11" spans="1:3" customHeight="1">
+        <x:v>64</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:3" ht="31.050000000000001" customHeight="1">
       <x:c r="A11" s="9">
         <x:v>9</x:v>
       </x:c>
       <x:c r="B11" s="8" t="s">
-        <x:v>39</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="C11" s="7" t="s">
-        <x:v>70</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="12" spans="1:3" customHeight="1">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:3" ht="31.050000000000001" customHeight="1">
       <x:c r="A12" s="9">
         <x:v>10</x:v>
       </x:c>
       <x:c r="B12" s="8" t="s">
-        <x:v>25</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="C12" s="7" t="s">
-        <x:v>63</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="13" spans="1:3" customHeight="1">
+        <x:v>53</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:3" ht="31.050000000000001" customHeight="1">
       <x:c r="A13" s="9">
         <x:v>11</x:v>
       </x:c>
       <x:c r="B13" s="8" t="s">
-        <x:v>53</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="C13" s="7" t="s">
-        <x:v>58</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="14" spans="1:3" customHeight="1">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:3" ht="31.050000000000001" customHeight="1">
       <x:c r="A14" s="9">
         <x:v>12</x:v>
       </x:c>
       <x:c r="B14" s="8" t="s">
-        <x:v>29</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="C14" s="7" t="s">
-        <x:v>43</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="15" spans="1:3" customHeight="1">
+        <x:v>30</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:3" ht="31.050000000000001" customHeight="1">
       <x:c r="A15" s="9">
         <x:v>13</x:v>
       </x:c>
       <x:c r="B15" s="8" t="s">
-        <x:v>24</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="C15" s="7" t="s">
-        <x:v>52</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="16" spans="1:3" customHeight="1">
+        <x:v>65</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:3" ht="31.050000000000001" customHeight="1">
       <x:c r="A16" s="9">
         <x:v>14</x:v>
       </x:c>
       <x:c r="B16" s="8" t="s">
-        <x:v>12</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="C16" s="7" t="s">
-        <x:v>46</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="17" spans="1:3" customHeight="1">
+        <x:v>73</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:3" ht="31.050000000000001" customHeight="1">
       <x:c r="A17" s="9">
         <x:v>15</x:v>
       </x:c>
       <x:c r="B17" s="8" t="s">
-        <x:v>4</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="C17" s="7" t="s">
-        <x:v>44</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="18" spans="1:3" customHeight="1">
+        <x:v>68</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:3" ht="31.050000000000001" customHeight="1">
       <x:c r="A18" s="9">
         <x:v>16</x:v>
       </x:c>
       <x:c r="B18" s="8" t="s">
-        <x:v>23</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="C18" s="7" t="s">
-        <x:v>48</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="19" spans="1:3" customHeight="1">
+        <x:v>66</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:3" ht="31.050000000000001" customHeight="1">
       <x:c r="A19" s="9">
         <x:v>17</x:v>
       </x:c>
       <x:c r="B19" s="8" t="s">
-        <x:v>13</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="C19" s="7" t="s">
-        <x:v>72</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="20" spans="1:3" customHeight="1">
+        <x:v>70</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:3" ht="31.050000000000001" customHeight="1">
       <x:c r="A20" s="9">
         <x:v>18</x:v>
       </x:c>
       <x:c r="B20" s="8" t="s">
-        <x:v>40</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="C20" s="7" t="s">
-        <x:v>45</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="21" spans="1:3" customHeight="1">
+        <x:v>56</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:3" ht="31.050000000000001" customHeight="1">
       <x:c r="A21" s="9">
         <x:v>19</x:v>
       </x:c>
       <x:c r="B21" s="8" t="s">
-        <x:v>11</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="C21" s="7" t="s">
-        <x:v>75</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="22" spans="1:3" customHeight="1">
+        <x:v>67</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:3" ht="31.050000000000001" customHeight="1">
       <x:c r="A22" s="9">
         <x:v>20</x:v>
       </x:c>
       <x:c r="B22" s="8" t="s">
-        <x:v>38</x:v>
-      </x:c>
-      <x:c r="C22" s="15" t="s">
-        <x:v>74</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="23" spans="1:3" customHeight="1">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C22" s="7" t="s">
+        <x:v>60</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:3" ht="31.050000000000001" customHeight="1">
       <x:c r="A23" s="9">
         <x:v>21</x:v>
       </x:c>
       <x:c r="B23" s="8" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="C23" s="16"/>
-    </x:row>
-    <x:row r="24" spans="1:3" customHeight="1">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C23" s="15" t="s">
+        <x:v>59</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:3" ht="31.050000000000001" customHeight="1">
       <x:c r="A24" s="9">
         <x:v>22</x:v>
       </x:c>
       <x:c r="B24" s="8" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="C24" s="15" t="s">
-        <x:v>19</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="25" spans="1:3" customHeight="1">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="C24" s="16"/>
+    </x:row>
+    <x:row r="25" spans="1:3" ht="31.050000000000001" customHeight="1">
       <x:c r="A25" s="9">
         <x:v>23</x:v>
       </x:c>
       <x:c r="B25" s="8" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="C25" s="16"/>
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="C25" s="15" t="s">
+        <x:v>47</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:3" ht="31.050000000000001" customHeight="1">
+      <x:c r="A26" s="9">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="B26" s="8" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="C26" s="16"/>
     </x:row>
   </x:sheetData>
   <x:mergeCells count="3">
     <x:mergeCell ref="A1:C1"/>
-    <x:mergeCell ref="C24:C25"/>
-    <x:mergeCell ref="C22:C23"/>
+    <x:mergeCell ref="C25:C26"/>
+    <x:mergeCell ref="C23:C24"/>
   </x:mergeCells>
-  <x:pageMargins left="0.69999998807907104" right="0.69999998807907104" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
+  <x:pageMargins left="0.69986110925674438" right="0.69986110925674438" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
   <x:pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="0" verticalDpi="0" copies="1"/>
 </x:worksheet>
 </file>
</xml_diff>